<commit_message>
added working import xls into dxf
</commit_message>
<xml_diff>
--- a/tests/test1/BOM_1.1_rev.xlsx
+++ b/tests/test1/BOM_1.1_rev.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ASETS-code\python\pyp-id_finder\tests\test1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8356487-7667-4555-8D5B-336CF2880031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DB5776-FF49-43B4-9C45-0F83134131FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="168">
   <si>
     <t>#</t>
   </si>
@@ -432,9 +432,6 @@
     <t>Ball Valve with Pneumatic actuator</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>XV501</t>
   </si>
   <si>
@@ -457,6 +454,96 @@
   </si>
   <si>
     <t>cartoncesso</t>
+  </si>
+  <si>
+    <t>AISI326</t>
+  </si>
+  <si>
+    <t>AISI336</t>
+  </si>
+  <si>
+    <t>AISI346</t>
+  </si>
+  <si>
+    <t>AISI317</t>
+  </si>
+  <si>
+    <t>AISI318</t>
+  </si>
+  <si>
+    <t>AISI319</t>
+  </si>
+  <si>
+    <t>AISI320</t>
+  </si>
+  <si>
+    <t>AISI321</t>
+  </si>
+  <si>
+    <t>AISI322</t>
+  </si>
+  <si>
+    <t>AISI323</t>
+  </si>
+  <si>
+    <t>AISI324</t>
+  </si>
+  <si>
+    <t>AISI325</t>
+  </si>
+  <si>
+    <t>AISI327</t>
+  </si>
+  <si>
+    <t>AISI328</t>
+  </si>
+  <si>
+    <t>AISI329</t>
+  </si>
+  <si>
+    <t>AISI330</t>
+  </si>
+  <si>
+    <t>AISI331</t>
+  </si>
+  <si>
+    <t>AISI332</t>
+  </si>
+  <si>
+    <t>AISI333</t>
+  </si>
+  <si>
+    <t>AISI334</t>
+  </si>
+  <si>
+    <t>AISI335</t>
+  </si>
+  <si>
+    <t>AISI337</t>
+  </si>
+  <si>
+    <t>AISI338</t>
+  </si>
+  <si>
+    <t>AISI339</t>
+  </si>
+  <si>
+    <t>AISI340</t>
+  </si>
+  <si>
+    <t>AISI341</t>
+  </si>
+  <si>
+    <t>AISI342</t>
+  </si>
+  <si>
+    <t>AISI343</t>
+  </si>
+  <si>
+    <t>AISI344</t>
+  </si>
+  <si>
+    <t>AISI345</t>
   </si>
 </sst>
 </file>
@@ -466,7 +553,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -550,6 +637,11 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -961,10 +1053,10 @@
   <dimension ref="A1:AH46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="L18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P37" sqref="P37"/>
+      <selection pane="bottomRight" activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1125,13 +1217,17 @@
       <c r="N2" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="28"/>
+      <c r="O2" s="28" t="s">
+        <v>112</v>
+      </c>
       <c r="P2" s="30"/>
       <c r="Q2" s="31"/>
       <c r="R2" s="28"/>
       <c r="S2" s="28"/>
       <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
+      <c r="U2" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V2" s="28"/>
       <c r="W2" s="28"/>
       <c r="X2" s="30"/>
@@ -1173,13 +1269,17 @@
       <c r="N3" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="O3" s="10"/>
+      <c r="O3" s="28" t="s">
+        <v>141</v>
+      </c>
       <c r="P3" s="13"/>
       <c r="Q3" s="18"/>
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
+      <c r="U3" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V3" s="10"/>
       <c r="W3" s="10"/>
       <c r="X3" s="13"/>
@@ -1221,13 +1321,17 @@
       <c r="N4" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="O4" s="10"/>
+      <c r="O4" s="28" t="s">
+        <v>142</v>
+      </c>
       <c r="P4" s="13"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
+      <c r="U4" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V4" s="10"/>
       <c r="W4" s="10"/>
       <c r="X4" s="13"/>
@@ -1269,13 +1373,17 @@
       <c r="N5" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="O5" s="10"/>
+      <c r="O5" s="28" t="s">
+        <v>143</v>
+      </c>
       <c r="P5" s="13"/>
       <c r="Q5" s="18"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
+      <c r="U5" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V5" s="10"/>
       <c r="W5" s="10"/>
       <c r="X5" s="13"/>
@@ -1317,13 +1425,17 @@
       <c r="N6" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="10"/>
+      <c r="O6" s="28" t="s">
+        <v>144</v>
+      </c>
       <c r="P6" s="13"/>
       <c r="Q6" s="18"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
+      <c r="U6" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V6" s="10"/>
       <c r="W6" s="10"/>
       <c r="X6" s="13"/>
@@ -1365,13 +1477,17 @@
       <c r="N7" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="O7" s="10"/>
+      <c r="O7" s="28" t="s">
+        <v>145</v>
+      </c>
       <c r="P7" s="13"/>
       <c r="Q7" s="18"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
+      <c r="U7" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V7" s="10"/>
       <c r="W7" s="10"/>
       <c r="X7" s="13"/>
@@ -1413,13 +1529,17 @@
       <c r="N8" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="O8" s="10"/>
+      <c r="O8" s="28" t="s">
+        <v>146</v>
+      </c>
       <c r="P8" s="13"/>
       <c r="Q8" s="18"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
+      <c r="U8" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
       <c r="X8" s="13"/>
@@ -1461,13 +1581,17 @@
       <c r="N9" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="O9" s="10"/>
+      <c r="O9" s="28" t="s">
+        <v>147</v>
+      </c>
       <c r="P9" s="13"/>
       <c r="Q9" s="18"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
+      <c r="U9" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
       <c r="X9" s="13"/>
@@ -1507,13 +1631,17 @@
         <v>53</v>
       </c>
       <c r="N10" s="13"/>
-      <c r="O10" s="10"/>
+      <c r="O10" s="28" t="s">
+        <v>148</v>
+      </c>
       <c r="P10" s="13"/>
       <c r="Q10" s="18"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
+      <c r="U10" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V10" s="10"/>
       <c r="W10" s="10"/>
       <c r="X10" s="13"/>
@@ -1555,13 +1683,17 @@
       <c r="N11" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="O11" s="10"/>
+      <c r="O11" s="28" t="s">
+        <v>149</v>
+      </c>
       <c r="P11" s="13"/>
       <c r="Q11" s="18"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
+      <c r="U11" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V11" s="10"/>
       <c r="W11" s="10"/>
       <c r="X11" s="13"/>
@@ -1603,13 +1735,17 @@
       <c r="N12" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="O12" s="10"/>
+      <c r="O12" s="28" t="s">
+        <v>138</v>
+      </c>
       <c r="P12" s="13"/>
       <c r="Q12" s="18"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
-      <c r="U12" s="10"/>
+      <c r="U12" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V12" s="10"/>
       <c r="W12" s="10"/>
       <c r="X12" s="13"/>
@@ -1651,13 +1787,17 @@
       <c r="N13" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="O13" s="10"/>
+      <c r="O13" s="28" t="s">
+        <v>150</v>
+      </c>
       <c r="P13" s="13"/>
       <c r="Q13" s="18"/>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
-      <c r="U13" s="10"/>
+      <c r="U13" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V13" s="10"/>
       <c r="W13" s="10"/>
       <c r="X13" s="13"/>
@@ -1699,13 +1839,17 @@
       <c r="N14" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="O14" s="10"/>
+      <c r="O14" s="28" t="s">
+        <v>151</v>
+      </c>
       <c r="P14" s="13"/>
       <c r="Q14" s="18"/>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
       <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
+      <c r="U14" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V14" s="10"/>
       <c r="W14" s="10"/>
       <c r="X14" s="13"/>
@@ -1747,13 +1891,17 @@
       <c r="N15" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="O15" s="10"/>
+      <c r="O15" s="28" t="s">
+        <v>152</v>
+      </c>
       <c r="P15" s="13"/>
       <c r="Q15" s="18"/>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
       <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
+      <c r="U15" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V15" s="10"/>
       <c r="W15" s="10"/>
       <c r="X15" s="13"/>
@@ -1795,13 +1943,17 @@
       <c r="N16" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="O16" s="10"/>
+      <c r="O16" s="28" t="s">
+        <v>153</v>
+      </c>
       <c r="P16" s="13"/>
       <c r="Q16" s="18"/>
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
       <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
+      <c r="U16" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V16" s="10"/>
       <c r="W16" s="10"/>
       <c r="X16" s="13"/>
@@ -1843,13 +1995,17 @@
       <c r="N17" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="O17" s="10"/>
+      <c r="O17" s="28" t="s">
+        <v>154</v>
+      </c>
       <c r="P17" s="13"/>
       <c r="Q17" s="18"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
       <c r="T17" s="10"/>
-      <c r="U17" s="10"/>
+      <c r="U17" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V17" s="10"/>
       <c r="W17" s="10"/>
       <c r="X17" s="13"/>
@@ -1891,13 +2047,17 @@
       <c r="N18" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="O18" s="10"/>
+      <c r="O18" s="28" t="s">
+        <v>155</v>
+      </c>
       <c r="P18" s="13"/>
       <c r="Q18" s="18"/>
       <c r="R18" s="10"/>
       <c r="S18" s="10"/>
       <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
+      <c r="U18" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V18" s="10"/>
       <c r="W18" s="10"/>
       <c r="X18" s="13"/>
@@ -1939,13 +2099,17 @@
       <c r="N19" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="O19" s="10"/>
+      <c r="O19" s="28" t="s">
+        <v>156</v>
+      </c>
       <c r="P19" s="13"/>
       <c r="Q19" s="18"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
-      <c r="U19" s="10"/>
+      <c r="U19" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V19" s="10"/>
       <c r="W19" s="10"/>
       <c r="X19" s="13"/>
@@ -1987,13 +2151,17 @@
       <c r="N20" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="O20" s="10"/>
+      <c r="O20" s="28" t="s">
+        <v>157</v>
+      </c>
       <c r="P20" s="13"/>
       <c r="Q20" s="18"/>
       <c r="R20" s="10"/>
       <c r="S20" s="10"/>
       <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
+      <c r="U20" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V20" s="10"/>
       <c r="W20" s="10"/>
       <c r="X20" s="13"/>
@@ -2035,13 +2203,17 @@
       <c r="N21" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="O21" s="10"/>
+      <c r="O21" s="28" t="s">
+        <v>158</v>
+      </c>
       <c r="P21" s="13"/>
       <c r="Q21" s="18"/>
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
       <c r="T21" s="10"/>
-      <c r="U21" s="10"/>
+      <c r="U21" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V21" s="10"/>
       <c r="W21" s="10"/>
       <c r="X21" s="13"/>
@@ -2083,13 +2255,17 @@
       <c r="N22" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="O22" s="10"/>
+      <c r="O22" s="28" t="s">
+        <v>139</v>
+      </c>
       <c r="P22" s="13"/>
       <c r="Q22" s="18"/>
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
       <c r="T22" s="10"/>
-      <c r="U22" s="10"/>
+      <c r="U22" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V22" s="10"/>
       <c r="W22" s="10"/>
       <c r="X22" s="13"/>
@@ -2129,13 +2305,17 @@
         <v>85</v>
       </c>
       <c r="N23" s="13"/>
-      <c r="O23" s="10"/>
+      <c r="O23" s="28" t="s">
+        <v>159</v>
+      </c>
       <c r="P23" s="13"/>
       <c r="Q23" s="18"/>
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
       <c r="T23" s="10"/>
-      <c r="U23" s="10"/>
+      <c r="U23" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V23" s="10"/>
       <c r="W23" s="10"/>
       <c r="X23" s="13"/>
@@ -2175,13 +2355,17 @@
         <v>85</v>
       </c>
       <c r="N24" s="13"/>
-      <c r="O24" s="10"/>
+      <c r="O24" s="28" t="s">
+        <v>160</v>
+      </c>
       <c r="P24" s="13"/>
       <c r="Q24" s="18"/>
       <c r="R24" s="10"/>
       <c r="S24" s="10"/>
       <c r="T24" s="10"/>
-      <c r="U24" s="10"/>
+      <c r="U24" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V24" s="10"/>
       <c r="W24" s="10"/>
       <c r="X24" s="13"/>
@@ -2221,13 +2405,17 @@
         <v>85</v>
       </c>
       <c r="N25" s="13"/>
-      <c r="O25" s="10"/>
+      <c r="O25" s="28" t="s">
+        <v>161</v>
+      </c>
       <c r="P25" s="13"/>
       <c r="Q25" s="18"/>
       <c r="R25" s="10"/>
       <c r="S25" s="10"/>
       <c r="T25" s="10"/>
-      <c r="U25" s="10"/>
+      <c r="U25" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V25" s="10"/>
       <c r="W25" s="10"/>
       <c r="X25" s="13"/>
@@ -2267,13 +2455,17 @@
         <v>85</v>
       </c>
       <c r="N26" s="13"/>
-      <c r="O26" s="10"/>
+      <c r="O26" s="28" t="s">
+        <v>162</v>
+      </c>
       <c r="P26" s="13"/>
       <c r="Q26" s="18"/>
       <c r="R26" s="10"/>
       <c r="S26" s="10"/>
       <c r="T26" s="10"/>
-      <c r="U26" s="10"/>
+      <c r="U26" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V26" s="10"/>
       <c r="W26" s="10"/>
       <c r="X26" s="13"/>
@@ -2313,13 +2505,17 @@
         <v>85</v>
       </c>
       <c r="N27" s="13"/>
-      <c r="O27" s="10"/>
+      <c r="O27" s="28" t="s">
+        <v>163</v>
+      </c>
       <c r="P27" s="13"/>
       <c r="Q27" s="18"/>
       <c r="R27" s="10"/>
       <c r="S27" s="10"/>
       <c r="T27" s="10"/>
-      <c r="U27" s="10"/>
+      <c r="U27" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V27" s="10"/>
       <c r="W27" s="10"/>
       <c r="X27" s="13"/>
@@ -2359,13 +2555,17 @@
         <v>85</v>
       </c>
       <c r="N28" s="13"/>
-      <c r="O28" s="10"/>
+      <c r="O28" s="28" t="s">
+        <v>164</v>
+      </c>
       <c r="P28" s="13"/>
       <c r="Q28" s="18"/>
       <c r="R28" s="10"/>
       <c r="S28" s="10"/>
       <c r="T28" s="10"/>
-      <c r="U28" s="10"/>
+      <c r="U28" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V28" s="10"/>
       <c r="W28" s="10"/>
       <c r="X28" s="13"/>
@@ -2405,13 +2605,17 @@
         <v>85</v>
       </c>
       <c r="N29" s="13"/>
-      <c r="O29" s="10"/>
+      <c r="O29" s="28" t="s">
+        <v>165</v>
+      </c>
       <c r="P29" s="13"/>
       <c r="Q29" s="18"/>
       <c r="R29" s="10"/>
       <c r="S29" s="10"/>
       <c r="T29" s="10"/>
-      <c r="U29" s="10"/>
+      <c r="U29" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V29" s="10"/>
       <c r="W29" s="10"/>
       <c r="X29" s="13"/>
@@ -2451,13 +2655,17 @@
         <v>85</v>
       </c>
       <c r="N30" s="13"/>
-      <c r="O30" s="10"/>
+      <c r="O30" s="28" t="s">
+        <v>166</v>
+      </c>
       <c r="P30" s="13"/>
       <c r="Q30" s="18"/>
       <c r="R30" s="10"/>
       <c r="S30" s="10"/>
       <c r="T30" s="10"/>
-      <c r="U30" s="10"/>
+      <c r="U30" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V30" s="10"/>
       <c r="W30" s="10"/>
       <c r="X30" s="13"/>
@@ -2497,13 +2705,17 @@
         <v>103</v>
       </c>
       <c r="N31" s="13"/>
-      <c r="O31" s="10"/>
+      <c r="O31" s="28" t="s">
+        <v>167</v>
+      </c>
       <c r="P31" s="13"/>
       <c r="Q31" s="18"/>
       <c r="R31" s="10"/>
       <c r="S31" s="10"/>
       <c r="T31" s="10"/>
-      <c r="U31" s="10"/>
+      <c r="U31" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V31" s="10"/>
       <c r="W31" s="10"/>
       <c r="X31" s="13"/>
@@ -2543,13 +2755,17 @@
         <v>103</v>
       </c>
       <c r="N32" s="13"/>
-      <c r="O32" s="10"/>
+      <c r="O32" s="28" t="s">
+        <v>140</v>
+      </c>
       <c r="P32" s="13"/>
       <c r="Q32" s="18"/>
       <c r="R32" s="10"/>
       <c r="S32" s="10"/>
       <c r="T32" s="10"/>
-      <c r="U32" s="10"/>
+      <c r="U32" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V32" s="10"/>
       <c r="W32" s="10"/>
       <c r="X32" s="13"/>
@@ -2755,20 +2971,20 @@
         <v>129</v>
       </c>
       <c r="N36" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="O36" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="O36" s="10" t="s">
+      <c r="P36" s="13" t="s">
         <v>137</v>
-      </c>
-      <c r="P36" s="13" t="s">
-        <v>138</v>
       </c>
       <c r="Q36" s="18"/>
       <c r="R36" s="10"/>
       <c r="S36" s="10"/>
       <c r="T36" s="10"/>
-      <c r="U36" s="10" t="s">
-        <v>130</v>
+      <c r="U36" s="11" t="s">
+        <v>133</v>
       </c>
       <c r="V36" s="10"/>
       <c r="W36" s="10"/>
@@ -2796,7 +3012,7 @@
       </c>
       <c r="D37" s="10"/>
       <c r="E37" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
@@ -2806,16 +3022,18 @@
       <c r="K37" s="10"/>
       <c r="L37" s="10"/>
       <c r="M37" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N37" s="13"/>
-      <c r="O37" s="10"/>
+      <c r="O37" s="11"/>
       <c r="P37" s="23"/>
       <c r="Q37" s="18"/>
       <c r="R37" s="10"/>
       <c r="S37" s="10"/>
       <c r="T37" s="10"/>
-      <c r="U37" s="10"/>
+      <c r="U37" s="11" t="s">
+        <v>133</v>
+      </c>
       <c r="V37" s="10"/>
       <c r="W37" s="10"/>
       <c r="X37" s="13"/>
@@ -2842,7 +3060,7 @@
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
@@ -2862,7 +3080,7 @@
       <c r="S38" s="11"/>
       <c r="T38" s="11"/>
       <c r="U38" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="V38" s="26"/>
       <c r="W38" s="11"/>
@@ -2889,7 +3107,7 @@
         <v>851</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M39" t="s">
         <v>129</v>
@@ -2917,9 +3135,10 @@
     <row r="46" spans="1:34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <autoFilter ref="A1:AJ38" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.78740157480314965" header="0" footer="0"/>
-  <pageSetup paperSize="8" orientation="landscape"/>
+  <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;LCommessa: C7084&amp;CImpianto &amp;R Date: marzo 2023</oddHeader>
     <oddFooter>&amp;LAQUAFIL &amp;C&amp;P /</oddFooter>

</xml_diff>